<commit_message>
some more minor changes
</commit_message>
<xml_diff>
--- a/CocoVille/Cost_EMI_Calculator.xlsx
+++ b/CocoVille/Cost_EMI_Calculator.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Cost and EMI Calculator" sheetId="1" r:id="rId3"/>
+    <sheet name="Cost and EMI Calculator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -100,35 +103,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$₹]#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -149,6 +158,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -163,6 +173,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -171,6 +182,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -181,6 +193,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -189,129 +202,371 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H995"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.43"/>
-    <col customWidth="1" min="2" max="2" width="11.14"/>
-    <col customWidth="1" min="3" max="3" width="2.71"/>
-    <col customWidth="1" min="5" max="5" width="15.71"/>
-    <col customWidth="1" min="6" max="6" width="3.86"/>
-    <col customWidth="1" min="7" max="7" width="16.57"/>
-    <col customWidth="1" min="8" max="8" width="13.0"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -325,7 +580,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -347,7 +602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -357,38 +612,38 @@
       <c r="G3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12" t="str">
+      <c r="H3" s="12">
         <f>E23*35%</f>
-        <v>₹1,254,640</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1254639.7849999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="14">
-        <v>1045.0</v>
+        <v>1045</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="16">
-        <v>2690.0</v>
-      </c>
-      <c r="E4" s="17" t="str">
+        <v>2690</v>
+      </c>
+      <c r="E4" s="17">
         <f>SUM(B4*D4)</f>
-        <v>₹2,811,050</v>
+        <v>2811050</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="18" t="str">
+      <c r="H4" s="18">
         <f>(E23-H3)/48</f>
-        <v>₹48,543</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>48542.610729166678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -398,24 +653,24 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="2"/>
       <c r="D6" s="20">
-        <v>79.0</v>
-      </c>
-      <c r="E6" s="17" t="str">
+        <v>79</v>
+      </c>
+      <c r="E6" s="17">
         <f>SUM(B4*D6)</f>
-        <v>₹82,555</v>
+        <v>82555</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -425,7 +680,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
@@ -433,13 +688,13 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="17">
-        <v>150000.0</v>
+        <v>150000</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -449,22 +704,22 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="17" t="str">
+      <c r="E10" s="17">
         <f>SUM(B4*2.5*12)</f>
-        <v>₹31,350</v>
+        <v>31350</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -474,7 +729,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
@@ -483,17 +738,17 @@
         <v>8</v>
       </c>
       <c r="D12" s="16">
-        <v>75.0</v>
-      </c>
-      <c r="E12" s="17" t="str">
+        <v>75</v>
+      </c>
+      <c r="E12" s="17">
         <f>SUM(B4*D12)</f>
-        <v>₹78,375</v>
+        <v>78375</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -503,7 +758,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
@@ -512,17 +767,17 @@
         <v>8</v>
       </c>
       <c r="D14" s="16">
-        <v>95.0</v>
-      </c>
-      <c r="E14" s="17" t="str">
+        <v>95</v>
+      </c>
+      <c r="E14" s="17">
         <f>SUM(B4*D14)</f>
-        <v>₹99,275</v>
+        <v>99275</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -532,22 +787,22 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="17" t="str">
+      <c r="E16" s="17">
         <f>SUM(E4+E6+E8)*5%</f>
-        <v>₹152,180</v>
+        <v>152180.25</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
@@ -557,7 +812,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>16</v>
       </c>
@@ -565,13 +820,13 @@
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="17">
-        <v>23000.0</v>
+        <v>23000</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -581,7 +836,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>17</v>
       </c>
@@ -589,13 +844,13 @@
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="17">
-        <v>15000.0</v>
+        <v>15000</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -605,129 +860,148 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="21" t="str">
+      <c r="B22" s="21">
         <f>SUM(E4:E12)</f>
-        <v>3,153,330</v>
+        <v>3153330</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="17" t="str">
+      <c r="E22" s="17">
         <f>SUM(B22*4.5%)</f>
-        <v>₹141,900</v>
+        <v>141899.85</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
-      <c r="E23" s="18" t="str">
+      <c r="E23" s="18">
         <f>SUM(E4:E22)</f>
-        <v>₹3,584,685</v>
+        <v>3584685.1</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
         <v>20</v>
       </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25">
-      <c r="A25" s="23" t="s">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
         <v>22</v>
       </c>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="4">
-        <v>3439030.0</v>
+        <f>E23</f>
+        <v>3584685.1</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="25">
-        <v>0.001</v>
-      </c>
-      <c r="E27" s="26" t="str">
-        <f t="shared" ref="E27:E30" si="1">B27*D27</f>
-        <v>₹3,439</v>
+        <v>1E-3</v>
+      </c>
+      <c r="E27" s="26">
+        <f t="shared" ref="E27:E30" si="0">B27*D27</f>
+        <v>3584.6851000000001</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="4">
-        <v>2850000.0</v>
+        <f>SUM(B4*2700+150000)</f>
+        <v>2971500</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="25">
-        <v>0.051</v>
-      </c>
-      <c r="E28" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>₹145,350</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E28" s="26">
+        <f t="shared" si="0"/>
+        <v>151546.5</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="4">
-        <v>2850000.0</v>
+        <f>SUM(B4*2700+150000)</f>
+        <v>2971500</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="25">
-        <v>0.005</v>
-      </c>
-      <c r="E29" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>₹14,250</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E29" s="26">
+        <f t="shared" si="0"/>
+        <v>14857.5</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="4">
-        <v>2850000.0</v>
+        <f>SUM(B4*2700+150000)</f>
+        <v>2971500</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>8</v>
@@ -735,2930 +1009,2931 @@
       <c r="D30" s="25">
         <v>0.01</v>
       </c>
-      <c r="E30" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>₹28,500</v>
+      <c r="E30" s="26">
+        <f t="shared" si="0"/>
+        <v>29715</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="30" t="s">
         <v>26</v>
       </c>
+      <c r="B31" s="31"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="26" t="str">
+      <c r="E31" s="26">
         <f>SUM(E27:E30)</f>
-        <v>₹191,539</v>
+        <v>199703.6851</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="28" t="str">
+      <c r="E32" s="28">
         <f>SUM(E23+E31)</f>
-        <v>₹3,776,224</v>
+        <v>3784388.7851</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="29"/>
     </row>
-    <row r="34">
+    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="29"/>
     </row>
-    <row r="35">
+    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F35" s="29"/>
     </row>
-    <row r="36">
+    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F36" s="29"/>
     </row>
-    <row r="37">
+    <row r="37" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F37" s="29"/>
     </row>
-    <row r="38">
+    <row r="38" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F38" s="29"/>
     </row>
-    <row r="39">
+    <row r="39" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F39" s="29"/>
     </row>
-    <row r="40">
+    <row r="40" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F40" s="29"/>
     </row>
-    <row r="41">
+    <row r="41" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F41" s="29"/>
     </row>
-    <row r="42">
+    <row r="42" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F42" s="29"/>
     </row>
-    <row r="43">
+    <row r="43" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F43" s="29"/>
     </row>
-    <row r="44">
+    <row r="44" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F44" s="29"/>
     </row>
-    <row r="45">
+    <row r="45" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F45" s="29"/>
     </row>
-    <row r="46">
+    <row r="46" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F46" s="29"/>
     </row>
-    <row r="47">
+    <row r="47" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F47" s="29"/>
     </row>
-    <row r="48">
+    <row r="48" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F48" s="29"/>
     </row>
-    <row r="49">
+    <row r="49" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F49" s="29"/>
     </row>
-    <row r="50">
+    <row r="50" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F50" s="29"/>
     </row>
-    <row r="51">
+    <row r="51" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F51" s="29"/>
     </row>
-    <row r="52">
+    <row r="52" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F52" s="29"/>
     </row>
-    <row r="53">
+    <row r="53" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F53" s="29"/>
     </row>
-    <row r="54">
+    <row r="54" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F54" s="29"/>
     </row>
-    <row r="55">
+    <row r="55" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F55" s="29"/>
     </row>
-    <row r="56">
+    <row r="56" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F56" s="29"/>
     </row>
-    <row r="57">
+    <row r="57" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F57" s="29"/>
     </row>
-    <row r="58">
+    <row r="58" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F58" s="29"/>
     </row>
-    <row r="59">
+    <row r="59" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F59" s="29"/>
     </row>
-    <row r="60">
+    <row r="60" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F60" s="29"/>
     </row>
-    <row r="61">
+    <row r="61" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="29"/>
     </row>
-    <row r="62">
+    <row r="62" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F62" s="29"/>
     </row>
-    <row r="63">
+    <row r="63" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F63" s="29"/>
     </row>
-    <row r="64">
+    <row r="64" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F64" s="29"/>
     </row>
-    <row r="65">
+    <row r="65" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F65" s="29"/>
     </row>
-    <row r="66">
+    <row r="66" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F66" s="29"/>
     </row>
-    <row r="67">
+    <row r="67" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F67" s="29"/>
     </row>
-    <row r="68">
+    <row r="68" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F68" s="29"/>
     </row>
-    <row r="69">
+    <row r="69" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F69" s="29"/>
     </row>
-    <row r="70">
+    <row r="70" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F70" s="29"/>
     </row>
-    <row r="71">
+    <row r="71" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F71" s="29"/>
     </row>
-    <row r="72">
+    <row r="72" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F72" s="29"/>
     </row>
-    <row r="73">
+    <row r="73" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F73" s="29"/>
     </row>
-    <row r="74">
+    <row r="74" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F74" s="29"/>
     </row>
-    <row r="75">
+    <row r="75" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F75" s="29"/>
     </row>
-    <row r="76">
+    <row r="76" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F76" s="29"/>
     </row>
-    <row r="77">
+    <row r="77" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F77" s="29"/>
     </row>
-    <row r="78">
+    <row r="78" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F78" s="29"/>
     </row>
-    <row r="79">
+    <row r="79" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F79" s="29"/>
     </row>
-    <row r="80">
+    <row r="80" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F80" s="29"/>
     </row>
-    <row r="81">
+    <row r="81" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F81" s="29"/>
     </row>
-    <row r="82">
+    <row r="82" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F82" s="29"/>
     </row>
-    <row r="83">
+    <row r="83" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F83" s="29"/>
     </row>
-    <row r="84">
+    <row r="84" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F84" s="29"/>
     </row>
-    <row r="85">
+    <row r="85" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F85" s="29"/>
     </row>
-    <row r="86">
+    <row r="86" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F86" s="29"/>
     </row>
-    <row r="87">
+    <row r="87" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F87" s="29"/>
     </row>
-    <row r="88">
+    <row r="88" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F88" s="29"/>
     </row>
-    <row r="89">
+    <row r="89" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F89" s="29"/>
     </row>
-    <row r="90">
+    <row r="90" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F90" s="29"/>
     </row>
-    <row r="91">
+    <row r="91" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F91" s="29"/>
     </row>
-    <row r="92">
+    <row r="92" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F92" s="29"/>
     </row>
-    <row r="93">
+    <row r="93" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F93" s="29"/>
     </row>
-    <row r="94">
+    <row r="94" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F94" s="29"/>
     </row>
-    <row r="95">
+    <row r="95" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F95" s="29"/>
     </row>
-    <row r="96">
+    <row r="96" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F96" s="29"/>
     </row>
-    <row r="97">
+    <row r="97" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F97" s="29"/>
     </row>
-    <row r="98">
+    <row r="98" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F98" s="29"/>
     </row>
-    <row r="99">
+    <row r="99" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F99" s="29"/>
     </row>
-    <row r="100">
+    <row r="100" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F100" s="29"/>
     </row>
-    <row r="101">
+    <row r="101" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F101" s="29"/>
     </row>
-    <row r="102">
+    <row r="102" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F102" s="29"/>
     </row>
-    <row r="103">
+    <row r="103" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F103" s="29"/>
     </row>
-    <row r="104">
+    <row r="104" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F104" s="29"/>
     </row>
-    <row r="105">
+    <row r="105" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F105" s="29"/>
     </row>
-    <row r="106">
+    <row r="106" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F106" s="29"/>
     </row>
-    <row r="107">
+    <row r="107" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F107" s="29"/>
     </row>
-    <row r="108">
+    <row r="108" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F108" s="29"/>
     </row>
-    <row r="109">
+    <row r="109" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F109" s="29"/>
     </row>
-    <row r="110">
+    <row r="110" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F110" s="29"/>
     </row>
-    <row r="111">
+    <row r="111" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F111" s="29"/>
     </row>
-    <row r="112">
+    <row r="112" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F112" s="29"/>
     </row>
-    <row r="113">
+    <row r="113" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F113" s="29"/>
     </row>
-    <row r="114">
+    <row r="114" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F114" s="29"/>
     </row>
-    <row r="115">
+    <row r="115" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F115" s="29"/>
     </row>
-    <row r="116">
+    <row r="116" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F116" s="29"/>
     </row>
-    <row r="117">
+    <row r="117" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F117" s="29"/>
     </row>
-    <row r="118">
+    <row r="118" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F118" s="29"/>
     </row>
-    <row r="119">
+    <row r="119" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F119" s="29"/>
     </row>
-    <row r="120">
+    <row r="120" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F120" s="29"/>
     </row>
-    <row r="121">
+    <row r="121" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F121" s="29"/>
     </row>
-    <row r="122">
+    <row r="122" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F122" s="29"/>
     </row>
-    <row r="123">
+    <row r="123" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F123" s="29"/>
     </row>
-    <row r="124">
+    <row r="124" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F124" s="29"/>
     </row>
-    <row r="125">
+    <row r="125" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F125" s="29"/>
     </row>
-    <row r="126">
+    <row r="126" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F126" s="29"/>
     </row>
-    <row r="127">
+    <row r="127" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F127" s="29"/>
     </row>
-    <row r="128">
+    <row r="128" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F128" s="29"/>
     </row>
-    <row r="129">
+    <row r="129" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F129" s="29"/>
     </row>
-    <row r="130">
+    <row r="130" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F130" s="29"/>
     </row>
-    <row r="131">
+    <row r="131" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F131" s="29"/>
     </row>
-    <row r="132">
+    <row r="132" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F132" s="29"/>
     </row>
-    <row r="133">
+    <row r="133" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F133" s="29"/>
     </row>
-    <row r="134">
+    <row r="134" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F134" s="29"/>
     </row>
-    <row r="135">
+    <row r="135" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F135" s="29"/>
     </row>
-    <row r="136">
+    <row r="136" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F136" s="29"/>
     </row>
-    <row r="137">
+    <row r="137" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F137" s="29"/>
     </row>
-    <row r="138">
+    <row r="138" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F138" s="29"/>
     </row>
-    <row r="139">
+    <row r="139" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F139" s="29"/>
     </row>
-    <row r="140">
+    <row r="140" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F140" s="29"/>
     </row>
-    <row r="141">
+    <row r="141" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F141" s="29"/>
     </row>
-    <row r="142">
+    <row r="142" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F142" s="29"/>
     </row>
-    <row r="143">
+    <row r="143" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F143" s="29"/>
     </row>
-    <row r="144">
+    <row r="144" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F144" s="29"/>
     </row>
-    <row r="145">
+    <row r="145" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F145" s="29"/>
     </row>
-    <row r="146">
+    <row r="146" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F146" s="29"/>
     </row>
-    <row r="147">
+    <row r="147" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F147" s="29"/>
     </row>
-    <row r="148">
+    <row r="148" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F148" s="29"/>
     </row>
-    <row r="149">
+    <row r="149" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F149" s="29"/>
     </row>
-    <row r="150">
+    <row r="150" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F150" s="29"/>
     </row>
-    <row r="151">
+    <row r="151" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F151" s="29"/>
     </row>
-    <row r="152">
+    <row r="152" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F152" s="29"/>
     </row>
-    <row r="153">
+    <row r="153" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F153" s="29"/>
     </row>
-    <row r="154">
+    <row r="154" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F154" s="29"/>
     </row>
-    <row r="155">
+    <row r="155" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F155" s="29"/>
     </row>
-    <row r="156">
+    <row r="156" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F156" s="29"/>
     </row>
-    <row r="157">
+    <row r="157" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F157" s="29"/>
     </row>
-    <row r="158">
+    <row r="158" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F158" s="29"/>
     </row>
-    <row r="159">
+    <row r="159" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F159" s="29"/>
     </row>
-    <row r="160">
+    <row r="160" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F160" s="29"/>
     </row>
-    <row r="161">
+    <row r="161" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F161" s="29"/>
     </row>
-    <row r="162">
+    <row r="162" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F162" s="29"/>
     </row>
-    <row r="163">
+    <row r="163" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F163" s="29"/>
     </row>
-    <row r="164">
+    <row r="164" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F164" s="29"/>
     </row>
-    <row r="165">
+    <row r="165" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F165" s="29"/>
     </row>
-    <row r="166">
+    <row r="166" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F166" s="29"/>
     </row>
-    <row r="167">
+    <row r="167" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F167" s="29"/>
     </row>
-    <row r="168">
+    <row r="168" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F168" s="29"/>
     </row>
-    <row r="169">
+    <row r="169" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F169" s="29"/>
     </row>
-    <row r="170">
+    <row r="170" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F170" s="29"/>
     </row>
-    <row r="171">
+    <row r="171" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F171" s="29"/>
     </row>
-    <row r="172">
+    <row r="172" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F172" s="29"/>
     </row>
-    <row r="173">
+    <row r="173" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F173" s="29"/>
     </row>
-    <row r="174">
+    <row r="174" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F174" s="29"/>
     </row>
-    <row r="175">
+    <row r="175" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F175" s="29"/>
     </row>
-    <row r="176">
+    <row r="176" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F176" s="29"/>
     </row>
-    <row r="177">
+    <row r="177" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F177" s="29"/>
     </row>
-    <row r="178">
+    <row r="178" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F178" s="29"/>
     </row>
-    <row r="179">
+    <row r="179" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F179" s="29"/>
     </row>
-    <row r="180">
+    <row r="180" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F180" s="29"/>
     </row>
-    <row r="181">
+    <row r="181" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F181" s="29"/>
     </row>
-    <row r="182">
+    <row r="182" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F182" s="29"/>
     </row>
-    <row r="183">
+    <row r="183" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F183" s="29"/>
     </row>
-    <row r="184">
+    <row r="184" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F184" s="29"/>
     </row>
-    <row r="185">
+    <row r="185" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F185" s="29"/>
     </row>
-    <row r="186">
+    <row r="186" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F186" s="29"/>
     </row>
-    <row r="187">
+    <row r="187" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F187" s="29"/>
     </row>
-    <row r="188">
+    <row r="188" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F188" s="29"/>
     </row>
-    <row r="189">
+    <row r="189" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F189" s="29"/>
     </row>
-    <row r="190">
+    <row r="190" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F190" s="29"/>
     </row>
-    <row r="191">
+    <row r="191" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F191" s="29"/>
     </row>
-    <row r="192">
+    <row r="192" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F192" s="29"/>
     </row>
-    <row r="193">
+    <row r="193" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F193" s="29"/>
     </row>
-    <row r="194">
+    <row r="194" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F194" s="29"/>
     </row>
-    <row r="195">
+    <row r="195" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F195" s="29"/>
     </row>
-    <row r="196">
+    <row r="196" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F196" s="29"/>
     </row>
-    <row r="197">
+    <row r="197" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F197" s="29"/>
     </row>
-    <row r="198">
+    <row r="198" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F198" s="29"/>
     </row>
-    <row r="199">
+    <row r="199" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F199" s="29"/>
     </row>
-    <row r="200">
+    <row r="200" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F200" s="29"/>
     </row>
-    <row r="201">
+    <row r="201" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F201" s="29"/>
     </row>
-    <row r="202">
+    <row r="202" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F202" s="29"/>
     </row>
-    <row r="203">
+    <row r="203" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F203" s="29"/>
     </row>
-    <row r="204">
+    <row r="204" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F204" s="29"/>
     </row>
-    <row r="205">
+    <row r="205" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F205" s="29"/>
     </row>
-    <row r="206">
+    <row r="206" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F206" s="29"/>
     </row>
-    <row r="207">
+    <row r="207" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F207" s="29"/>
     </row>
-    <row r="208">
+    <row r="208" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F208" s="29"/>
     </row>
-    <row r="209">
+    <row r="209" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F209" s="29"/>
     </row>
-    <row r="210">
+    <row r="210" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F210" s="29"/>
     </row>
-    <row r="211">
+    <row r="211" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F211" s="29"/>
     </row>
-    <row r="212">
+    <row r="212" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F212" s="29"/>
     </row>
-    <row r="213">
+    <row r="213" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F213" s="29"/>
     </row>
-    <row r="214">
+    <row r="214" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F214" s="29"/>
     </row>
-    <row r="215">
+    <row r="215" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F215" s="29"/>
     </row>
-    <row r="216">
+    <row r="216" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F216" s="29"/>
     </row>
-    <row r="217">
+    <row r="217" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F217" s="29"/>
     </row>
-    <row r="218">
+    <row r="218" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F218" s="29"/>
     </row>
-    <row r="219">
+    <row r="219" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F219" s="29"/>
     </row>
-    <row r="220">
+    <row r="220" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F220" s="29"/>
     </row>
-    <row r="221">
+    <row r="221" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F221" s="29"/>
     </row>
-    <row r="222">
+    <row r="222" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F222" s="29"/>
     </row>
-    <row r="223">
+    <row r="223" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F223" s="29"/>
     </row>
-    <row r="224">
+    <row r="224" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F224" s="29"/>
     </row>
-    <row r="225">
+    <row r="225" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F225" s="29"/>
     </row>
-    <row r="226">
+    <row r="226" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F226" s="29"/>
     </row>
-    <row r="227">
+    <row r="227" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F227" s="29"/>
     </row>
-    <row r="228">
+    <row r="228" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F228" s="29"/>
     </row>
-    <row r="229">
+    <row r="229" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F229" s="29"/>
     </row>
-    <row r="230">
+    <row r="230" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F230" s="29"/>
     </row>
-    <row r="231">
+    <row r="231" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F231" s="29"/>
     </row>
-    <row r="232">
+    <row r="232" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F232" s="29"/>
     </row>
-    <row r="233">
+    <row r="233" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F233" s="29"/>
     </row>
-    <row r="234">
+    <row r="234" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F234" s="29"/>
     </row>
-    <row r="235">
+    <row r="235" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F235" s="29"/>
     </row>
-    <row r="236">
+    <row r="236" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F236" s="29"/>
     </row>
-    <row r="237">
+    <row r="237" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F237" s="29"/>
     </row>
-    <row r="238">
+    <row r="238" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F238" s="29"/>
     </row>
-    <row r="239">
+    <row r="239" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F239" s="29"/>
     </row>
-    <row r="240">
+    <row r="240" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F240" s="29"/>
     </row>
-    <row r="241">
+    <row r="241" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F241" s="29"/>
     </row>
-    <row r="242">
+    <row r="242" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F242" s="29"/>
     </row>
-    <row r="243">
+    <row r="243" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F243" s="29"/>
     </row>
-    <row r="244">
+    <row r="244" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F244" s="29"/>
     </row>
-    <row r="245">
+    <row r="245" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F245" s="29"/>
     </row>
-    <row r="246">
+    <row r="246" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F246" s="29"/>
     </row>
-    <row r="247">
+    <row r="247" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F247" s="29"/>
     </row>
-    <row r="248">
+    <row r="248" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F248" s="29"/>
     </row>
-    <row r="249">
+    <row r="249" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F249" s="29"/>
     </row>
-    <row r="250">
+    <row r="250" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F250" s="29"/>
     </row>
-    <row r="251">
+    <row r="251" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F251" s="29"/>
     </row>
-    <row r="252">
+    <row r="252" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F252" s="29"/>
     </row>
-    <row r="253">
+    <row r="253" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F253" s="29"/>
     </row>
-    <row r="254">
+    <row r="254" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F254" s="29"/>
     </row>
-    <row r="255">
+    <row r="255" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F255" s="29"/>
     </row>
-    <row r="256">
+    <row r="256" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F256" s="29"/>
     </row>
-    <row r="257">
+    <row r="257" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F257" s="29"/>
     </row>
-    <row r="258">
+    <row r="258" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F258" s="29"/>
     </row>
-    <row r="259">
+    <row r="259" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F259" s="29"/>
     </row>
-    <row r="260">
+    <row r="260" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F260" s="29"/>
     </row>
-    <row r="261">
+    <row r="261" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F261" s="29"/>
     </row>
-    <row r="262">
+    <row r="262" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F262" s="29"/>
     </row>
-    <row r="263">
+    <row r="263" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F263" s="29"/>
     </row>
-    <row r="264">
+    <row r="264" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F264" s="29"/>
     </row>
-    <row r="265">
+    <row r="265" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F265" s="29"/>
     </row>
-    <row r="266">
+    <row r="266" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F266" s="29"/>
     </row>
-    <row r="267">
+    <row r="267" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F267" s="29"/>
     </row>
-    <row r="268">
+    <row r="268" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F268" s="29"/>
     </row>
-    <row r="269">
+    <row r="269" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F269" s="29"/>
     </row>
-    <row r="270">
+    <row r="270" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F270" s="29"/>
     </row>
-    <row r="271">
+    <row r="271" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F271" s="29"/>
     </row>
-    <row r="272">
+    <row r="272" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F272" s="29"/>
     </row>
-    <row r="273">
+    <row r="273" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F273" s="29"/>
     </row>
-    <row r="274">
+    <row r="274" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F274" s="29"/>
     </row>
-    <row r="275">
+    <row r="275" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F275" s="29"/>
     </row>
-    <row r="276">
+    <row r="276" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F276" s="29"/>
     </row>
-    <row r="277">
+    <row r="277" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F277" s="29"/>
     </row>
-    <row r="278">
+    <row r="278" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F278" s="29"/>
     </row>
-    <row r="279">
+    <row r="279" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F279" s="29"/>
     </row>
-    <row r="280">
+    <row r="280" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F280" s="29"/>
     </row>
-    <row r="281">
+    <row r="281" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F281" s="29"/>
     </row>
-    <row r="282">
+    <row r="282" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F282" s="29"/>
     </row>
-    <row r="283">
+    <row r="283" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F283" s="29"/>
     </row>
-    <row r="284">
+    <row r="284" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F284" s="29"/>
     </row>
-    <row r="285">
+    <row r="285" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F285" s="29"/>
     </row>
-    <row r="286">
+    <row r="286" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F286" s="29"/>
     </row>
-    <row r="287">
+    <row r="287" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F287" s="29"/>
     </row>
-    <row r="288">
+    <row r="288" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F288" s="29"/>
     </row>
-    <row r="289">
+    <row r="289" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F289" s="29"/>
     </row>
-    <row r="290">
+    <row r="290" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F290" s="29"/>
     </row>
-    <row r="291">
+    <row r="291" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F291" s="29"/>
     </row>
-    <row r="292">
+    <row r="292" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F292" s="29"/>
     </row>
-    <row r="293">
+    <row r="293" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F293" s="29"/>
     </row>
-    <row r="294">
+    <row r="294" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F294" s="29"/>
     </row>
-    <row r="295">
+    <row r="295" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F295" s="29"/>
     </row>
-    <row r="296">
+    <row r="296" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F296" s="29"/>
     </row>
-    <row r="297">
+    <row r="297" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F297" s="29"/>
     </row>
-    <row r="298">
+    <row r="298" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F298" s="29"/>
     </row>
-    <row r="299">
+    <row r="299" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F299" s="29"/>
     </row>
-    <row r="300">
+    <row r="300" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F300" s="29"/>
     </row>
-    <row r="301">
+    <row r="301" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F301" s="29"/>
     </row>
-    <row r="302">
+    <row r="302" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F302" s="29"/>
     </row>
-    <row r="303">
+    <row r="303" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F303" s="29"/>
     </row>
-    <row r="304">
+    <row r="304" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F304" s="29"/>
     </row>
-    <row r="305">
+    <row r="305" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F305" s="29"/>
     </row>
-    <row r="306">
+    <row r="306" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F306" s="29"/>
     </row>
-    <row r="307">
+    <row r="307" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F307" s="29"/>
     </row>
-    <row r="308">
+    <row r="308" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F308" s="29"/>
     </row>
-    <row r="309">
+    <row r="309" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F309" s="29"/>
     </row>
-    <row r="310">
+    <row r="310" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F310" s="29"/>
     </row>
-    <row r="311">
+    <row r="311" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F311" s="29"/>
     </row>
-    <row r="312">
+    <row r="312" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F312" s="29"/>
     </row>
-    <row r="313">
+    <row r="313" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F313" s="29"/>
     </row>
-    <row r="314">
+    <row r="314" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F314" s="29"/>
     </row>
-    <row r="315">
+    <row r="315" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F315" s="29"/>
     </row>
-    <row r="316">
+    <row r="316" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F316" s="29"/>
     </row>
-    <row r="317">
+    <row r="317" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F317" s="29"/>
     </row>
-    <row r="318">
+    <row r="318" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F318" s="29"/>
     </row>
-    <row r="319">
+    <row r="319" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F319" s="29"/>
     </row>
-    <row r="320">
+    <row r="320" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F320" s="29"/>
     </row>
-    <row r="321">
+    <row r="321" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F321" s="29"/>
     </row>
-    <row r="322">
+    <row r="322" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F322" s="29"/>
     </row>
-    <row r="323">
+    <row r="323" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F323" s="29"/>
     </row>
-    <row r="324">
+    <row r="324" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F324" s="29"/>
     </row>
-    <row r="325">
+    <row r="325" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F325" s="29"/>
     </row>
-    <row r="326">
+    <row r="326" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F326" s="29"/>
     </row>
-    <row r="327">
+    <row r="327" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F327" s="29"/>
     </row>
-    <row r="328">
+    <row r="328" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F328" s="29"/>
     </row>
-    <row r="329">
+    <row r="329" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F329" s="29"/>
     </row>
-    <row r="330">
+    <row r="330" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F330" s="29"/>
     </row>
-    <row r="331">
+    <row r="331" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F331" s="29"/>
     </row>
-    <row r="332">
+    <row r="332" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F332" s="29"/>
     </row>
-    <row r="333">
+    <row r="333" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F333" s="29"/>
     </row>
-    <row r="334">
+    <row r="334" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F334" s="29"/>
     </row>
-    <row r="335">
+    <row r="335" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F335" s="29"/>
     </row>
-    <row r="336">
+    <row r="336" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F336" s="29"/>
     </row>
-    <row r="337">
+    <row r="337" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F337" s="29"/>
     </row>
-    <row r="338">
+    <row r="338" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F338" s="29"/>
     </row>
-    <row r="339">
+    <row r="339" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F339" s="29"/>
     </row>
-    <row r="340">
+    <row r="340" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F340" s="29"/>
     </row>
-    <row r="341">
+    <row r="341" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F341" s="29"/>
     </row>
-    <row r="342">
+    <row r="342" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F342" s="29"/>
     </row>
-    <row r="343">
+    <row r="343" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F343" s="29"/>
     </row>
-    <row r="344">
+    <row r="344" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F344" s="29"/>
     </row>
-    <row r="345">
+    <row r="345" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F345" s="29"/>
     </row>
-    <row r="346">
+    <row r="346" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F346" s="29"/>
     </row>
-    <row r="347">
+    <row r="347" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F347" s="29"/>
     </row>
-    <row r="348">
+    <row r="348" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F348" s="29"/>
     </row>
-    <row r="349">
+    <row r="349" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F349" s="29"/>
     </row>
-    <row r="350">
+    <row r="350" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F350" s="29"/>
     </row>
-    <row r="351">
+    <row r="351" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F351" s="29"/>
     </row>
-    <row r="352">
+    <row r="352" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F352" s="29"/>
     </row>
-    <row r="353">
+    <row r="353" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F353" s="29"/>
     </row>
-    <row r="354">
+    <row r="354" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F354" s="29"/>
     </row>
-    <row r="355">
+    <row r="355" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F355" s="29"/>
     </row>
-    <row r="356">
+    <row r="356" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F356" s="29"/>
     </row>
-    <row r="357">
+    <row r="357" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F357" s="29"/>
     </row>
-    <row r="358">
+    <row r="358" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F358" s="29"/>
     </row>
-    <row r="359">
+    <row r="359" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F359" s="29"/>
     </row>
-    <row r="360">
+    <row r="360" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F360" s="29"/>
     </row>
-    <row r="361">
+    <row r="361" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F361" s="29"/>
     </row>
-    <row r="362">
+    <row r="362" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F362" s="29"/>
     </row>
-    <row r="363">
+    <row r="363" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F363" s="29"/>
     </row>
-    <row r="364">
+    <row r="364" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F364" s="29"/>
     </row>
-    <row r="365">
+    <row r="365" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F365" s="29"/>
     </row>
-    <row r="366">
+    <row r="366" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F366" s="29"/>
     </row>
-    <row r="367">
+    <row r="367" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F367" s="29"/>
     </row>
-    <row r="368">
+    <row r="368" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F368" s="29"/>
     </row>
-    <row r="369">
+    <row r="369" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F369" s="29"/>
     </row>
-    <row r="370">
+    <row r="370" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F370" s="29"/>
     </row>
-    <row r="371">
+    <row r="371" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F371" s="29"/>
     </row>
-    <row r="372">
+    <row r="372" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F372" s="29"/>
     </row>
-    <row r="373">
+    <row r="373" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F373" s="29"/>
     </row>
-    <row r="374">
+    <row r="374" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F374" s="29"/>
     </row>
-    <row r="375">
+    <row r="375" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F375" s="29"/>
     </row>
-    <row r="376">
+    <row r="376" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F376" s="29"/>
     </row>
-    <row r="377">
+    <row r="377" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F377" s="29"/>
     </row>
-    <row r="378">
+    <row r="378" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F378" s="29"/>
     </row>
-    <row r="379">
+    <row r="379" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F379" s="29"/>
     </row>
-    <row r="380">
+    <row r="380" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F380" s="29"/>
     </row>
-    <row r="381">
+    <row r="381" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F381" s="29"/>
     </row>
-    <row r="382">
+    <row r="382" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F382" s="29"/>
     </row>
-    <row r="383">
+    <row r="383" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F383" s="29"/>
     </row>
-    <row r="384">
+    <row r="384" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F384" s="29"/>
     </row>
-    <row r="385">
+    <row r="385" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F385" s="29"/>
     </row>
-    <row r="386">
+    <row r="386" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F386" s="29"/>
     </row>
-    <row r="387">
+    <row r="387" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F387" s="29"/>
     </row>
-    <row r="388">
+    <row r="388" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F388" s="29"/>
     </row>
-    <row r="389">
+    <row r="389" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F389" s="29"/>
     </row>
-    <row r="390">
+    <row r="390" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F390" s="29"/>
     </row>
-    <row r="391">
+    <row r="391" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F391" s="29"/>
     </row>
-    <row r="392">
+    <row r="392" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F392" s="29"/>
     </row>
-    <row r="393">
+    <row r="393" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F393" s="29"/>
     </row>
-    <row r="394">
+    <row r="394" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F394" s="29"/>
     </row>
-    <row r="395">
+    <row r="395" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F395" s="29"/>
     </row>
-    <row r="396">
+    <row r="396" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F396" s="29"/>
     </row>
-    <row r="397">
+    <row r="397" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F397" s="29"/>
     </row>
-    <row r="398">
+    <row r="398" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F398" s="29"/>
     </row>
-    <row r="399">
+    <row r="399" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F399" s="29"/>
     </row>
-    <row r="400">
+    <row r="400" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F400" s="29"/>
     </row>
-    <row r="401">
+    <row r="401" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F401" s="29"/>
     </row>
-    <row r="402">
+    <row r="402" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F402" s="29"/>
     </row>
-    <row r="403">
+    <row r="403" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F403" s="29"/>
     </row>
-    <row r="404">
+    <row r="404" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F404" s="29"/>
     </row>
-    <row r="405">
+    <row r="405" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F405" s="29"/>
     </row>
-    <row r="406">
+    <row r="406" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F406" s="29"/>
     </row>
-    <row r="407">
+    <row r="407" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F407" s="29"/>
     </row>
-    <row r="408">
+    <row r="408" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F408" s="29"/>
     </row>
-    <row r="409">
+    <row r="409" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F409" s="29"/>
     </row>
-    <row r="410">
+    <row r="410" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F410" s="29"/>
     </row>
-    <row r="411">
+    <row r="411" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F411" s="29"/>
     </row>
-    <row r="412">
+    <row r="412" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F412" s="29"/>
     </row>
-    <row r="413">
+    <row r="413" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F413" s="29"/>
     </row>
-    <row r="414">
+    <row r="414" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F414" s="29"/>
     </row>
-    <row r="415">
+    <row r="415" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F415" s="29"/>
     </row>
-    <row r="416">
+    <row r="416" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F416" s="29"/>
     </row>
-    <row r="417">
+    <row r="417" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F417" s="29"/>
     </row>
-    <row r="418">
+    <row r="418" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F418" s="29"/>
     </row>
-    <row r="419">
+    <row r="419" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F419" s="29"/>
     </row>
-    <row r="420">
+    <row r="420" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F420" s="29"/>
     </row>
-    <row r="421">
+    <row r="421" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F421" s="29"/>
     </row>
-    <row r="422">
+    <row r="422" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F422" s="29"/>
     </row>
-    <row r="423">
+    <row r="423" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F423" s="29"/>
     </row>
-    <row r="424">
+    <row r="424" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F424" s="29"/>
     </row>
-    <row r="425">
+    <row r="425" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F425" s="29"/>
     </row>
-    <row r="426">
+    <row r="426" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F426" s="29"/>
     </row>
-    <row r="427">
+    <row r="427" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F427" s="29"/>
     </row>
-    <row r="428">
+    <row r="428" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F428" s="29"/>
     </row>
-    <row r="429">
+    <row r="429" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F429" s="29"/>
     </row>
-    <row r="430">
+    <row r="430" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F430" s="29"/>
     </row>
-    <row r="431">
+    <row r="431" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F431" s="29"/>
     </row>
-    <row r="432">
+    <row r="432" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F432" s="29"/>
     </row>
-    <row r="433">
+    <row r="433" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F433" s="29"/>
     </row>
-    <row r="434">
+    <row r="434" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F434" s="29"/>
     </row>
-    <row r="435">
+    <row r="435" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F435" s="29"/>
     </row>
-    <row r="436">
+    <row r="436" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F436" s="29"/>
     </row>
-    <row r="437">
+    <row r="437" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F437" s="29"/>
     </row>
-    <row r="438">
+    <row r="438" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F438" s="29"/>
     </row>
-    <row r="439">
+    <row r="439" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F439" s="29"/>
     </row>
-    <row r="440">
+    <row r="440" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F440" s="29"/>
     </row>
-    <row r="441">
+    <row r="441" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F441" s="29"/>
     </row>
-    <row r="442">
+    <row r="442" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F442" s="29"/>
     </row>
-    <row r="443">
+    <row r="443" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F443" s="29"/>
     </row>
-    <row r="444">
+    <row r="444" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F444" s="29"/>
     </row>
-    <row r="445">
+    <row r="445" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F445" s="29"/>
     </row>
-    <row r="446">
+    <row r="446" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F446" s="29"/>
     </row>
-    <row r="447">
+    <row r="447" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F447" s="29"/>
     </row>
-    <row r="448">
+    <row r="448" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F448" s="29"/>
     </row>
-    <row r="449">
+    <row r="449" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F449" s="29"/>
     </row>
-    <row r="450">
+    <row r="450" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F450" s="29"/>
     </row>
-    <row r="451">
+    <row r="451" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F451" s="29"/>
     </row>
-    <row r="452">
+    <row r="452" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F452" s="29"/>
     </row>
-    <row r="453">
+    <row r="453" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F453" s="29"/>
     </row>
-    <row r="454">
+    <row r="454" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F454" s="29"/>
     </row>
-    <row r="455">
+    <row r="455" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F455" s="29"/>
     </row>
-    <row r="456">
+    <row r="456" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F456" s="29"/>
     </row>
-    <row r="457">
+    <row r="457" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F457" s="29"/>
     </row>
-    <row r="458">
+    <row r="458" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F458" s="29"/>
     </row>
-    <row r="459">
+    <row r="459" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F459" s="29"/>
     </row>
-    <row r="460">
+    <row r="460" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F460" s="29"/>
     </row>
-    <row r="461">
+    <row r="461" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F461" s="29"/>
     </row>
-    <row r="462">
+    <row r="462" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F462" s="29"/>
     </row>
-    <row r="463">
+    <row r="463" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F463" s="29"/>
     </row>
-    <row r="464">
+    <row r="464" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F464" s="29"/>
     </row>
-    <row r="465">
+    <row r="465" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F465" s="29"/>
     </row>
-    <row r="466">
+    <row r="466" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F466" s="29"/>
     </row>
-    <row r="467">
+    <row r="467" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F467" s="29"/>
     </row>
-    <row r="468">
+    <row r="468" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F468" s="29"/>
     </row>
-    <row r="469">
+    <row r="469" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F469" s="29"/>
     </row>
-    <row r="470">
+    <row r="470" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F470" s="29"/>
     </row>
-    <row r="471">
+    <row r="471" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F471" s="29"/>
     </row>
-    <row r="472">
+    <row r="472" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F472" s="29"/>
     </row>
-    <row r="473">
+    <row r="473" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F473" s="29"/>
     </row>
-    <row r="474">
+    <row r="474" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F474" s="29"/>
     </row>
-    <row r="475">
+    <row r="475" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F475" s="29"/>
     </row>
-    <row r="476">
+    <row r="476" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F476" s="29"/>
     </row>
-    <row r="477">
+    <row r="477" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F477" s="29"/>
     </row>
-    <row r="478">
+    <row r="478" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F478" s="29"/>
     </row>
-    <row r="479">
+    <row r="479" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F479" s="29"/>
     </row>
-    <row r="480">
+    <row r="480" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F480" s="29"/>
     </row>
-    <row r="481">
+    <row r="481" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F481" s="29"/>
     </row>
-    <row r="482">
+    <row r="482" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F482" s="29"/>
     </row>
-    <row r="483">
+    <row r="483" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F483" s="29"/>
     </row>
-    <row r="484">
+    <row r="484" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F484" s="29"/>
     </row>
-    <row r="485">
+    <row r="485" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F485" s="29"/>
     </row>
-    <row r="486">
+    <row r="486" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F486" s="29"/>
     </row>
-    <row r="487">
+    <row r="487" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F487" s="29"/>
     </row>
-    <row r="488">
+    <row r="488" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F488" s="29"/>
     </row>
-    <row r="489">
+    <row r="489" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F489" s="29"/>
     </row>
-    <row r="490">
+    <row r="490" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F490" s="29"/>
     </row>
-    <row r="491">
+    <row r="491" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F491" s="29"/>
     </row>
-    <row r="492">
+    <row r="492" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F492" s="29"/>
     </row>
-    <row r="493">
+    <row r="493" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F493" s="29"/>
     </row>
-    <row r="494">
+    <row r="494" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F494" s="29"/>
     </row>
-    <row r="495">
+    <row r="495" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F495" s="29"/>
     </row>
-    <row r="496">
+    <row r="496" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F496" s="29"/>
     </row>
-    <row r="497">
+    <row r="497" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F497" s="29"/>
     </row>
-    <row r="498">
+    <row r="498" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F498" s="29"/>
     </row>
-    <row r="499">
+    <row r="499" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F499" s="29"/>
     </row>
-    <row r="500">
+    <row r="500" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F500" s="29"/>
     </row>
-    <row r="501">
+    <row r="501" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F501" s="29"/>
     </row>
-    <row r="502">
+    <row r="502" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F502" s="29"/>
     </row>
-    <row r="503">
+    <row r="503" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F503" s="29"/>
     </row>
-    <row r="504">
+    <row r="504" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F504" s="29"/>
     </row>
-    <row r="505">
+    <row r="505" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F505" s="29"/>
     </row>
-    <row r="506">
+    <row r="506" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F506" s="29"/>
     </row>
-    <row r="507">
+    <row r="507" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F507" s="29"/>
     </row>
-    <row r="508">
+    <row r="508" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F508" s="29"/>
     </row>
-    <row r="509">
+    <row r="509" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F509" s="29"/>
     </row>
-    <row r="510">
+    <row r="510" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F510" s="29"/>
     </row>
-    <row r="511">
+    <row r="511" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F511" s="29"/>
     </row>
-    <row r="512">
+    <row r="512" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F512" s="29"/>
     </row>
-    <row r="513">
+    <row r="513" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F513" s="29"/>
     </row>
-    <row r="514">
+    <row r="514" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F514" s="29"/>
     </row>
-    <row r="515">
+    <row r="515" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F515" s="29"/>
     </row>
-    <row r="516">
+    <row r="516" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F516" s="29"/>
     </row>
-    <row r="517">
+    <row r="517" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F517" s="29"/>
     </row>
-    <row r="518">
+    <row r="518" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F518" s="29"/>
     </row>
-    <row r="519">
+    <row r="519" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F519" s="29"/>
     </row>
-    <row r="520">
+    <row r="520" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F520" s="29"/>
     </row>
-    <row r="521">
+    <row r="521" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F521" s="29"/>
     </row>
-    <row r="522">
+    <row r="522" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F522" s="29"/>
     </row>
-    <row r="523">
+    <row r="523" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F523" s="29"/>
     </row>
-    <row r="524">
+    <row r="524" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F524" s="29"/>
     </row>
-    <row r="525">
+    <row r="525" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F525" s="29"/>
     </row>
-    <row r="526">
+    <row r="526" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F526" s="29"/>
     </row>
-    <row r="527">
+    <row r="527" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F527" s="29"/>
     </row>
-    <row r="528">
+    <row r="528" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F528" s="29"/>
     </row>
-    <row r="529">
+    <row r="529" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F529" s="29"/>
     </row>
-    <row r="530">
+    <row r="530" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F530" s="29"/>
     </row>
-    <row r="531">
+    <row r="531" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F531" s="29"/>
     </row>
-    <row r="532">
+    <row r="532" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F532" s="29"/>
     </row>
-    <row r="533">
+    <row r="533" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F533" s="29"/>
     </row>
-    <row r="534">
+    <row r="534" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F534" s="29"/>
     </row>
-    <row r="535">
+    <row r="535" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F535" s="29"/>
     </row>
-    <row r="536">
+    <row r="536" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F536" s="29"/>
     </row>
-    <row r="537">
+    <row r="537" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F537" s="29"/>
     </row>
-    <row r="538">
+    <row r="538" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F538" s="29"/>
     </row>
-    <row r="539">
+    <row r="539" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F539" s="29"/>
     </row>
-    <row r="540">
+    <row r="540" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F540" s="29"/>
     </row>
-    <row r="541">
+    <row r="541" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F541" s="29"/>
     </row>
-    <row r="542">
+    <row r="542" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F542" s="29"/>
     </row>
-    <row r="543">
+    <row r="543" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F543" s="29"/>
     </row>
-    <row r="544">
+    <row r="544" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F544" s="29"/>
     </row>
-    <row r="545">
+    <row r="545" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F545" s="29"/>
     </row>
-    <row r="546">
+    <row r="546" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F546" s="29"/>
     </row>
-    <row r="547">
+    <row r="547" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F547" s="29"/>
     </row>
-    <row r="548">
+    <row r="548" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F548" s="29"/>
     </row>
-    <row r="549">
+    <row r="549" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F549" s="29"/>
     </row>
-    <row r="550">
+    <row r="550" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F550" s="29"/>
     </row>
-    <row r="551">
+    <row r="551" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F551" s="29"/>
     </row>
-    <row r="552">
+    <row r="552" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F552" s="29"/>
     </row>
-    <row r="553">
+    <row r="553" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F553" s="29"/>
     </row>
-    <row r="554">
+    <row r="554" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F554" s="29"/>
     </row>
-    <row r="555">
+    <row r="555" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F555" s="29"/>
     </row>
-    <row r="556">
+    <row r="556" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F556" s="29"/>
     </row>
-    <row r="557">
+    <row r="557" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F557" s="29"/>
     </row>
-    <row r="558">
+    <row r="558" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F558" s="29"/>
     </row>
-    <row r="559">
+    <row r="559" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F559" s="29"/>
     </row>
-    <row r="560">
+    <row r="560" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F560" s="29"/>
     </row>
-    <row r="561">
+    <row r="561" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F561" s="29"/>
     </row>
-    <row r="562">
+    <row r="562" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F562" s="29"/>
     </row>
-    <row r="563">
+    <row r="563" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F563" s="29"/>
     </row>
-    <row r="564">
+    <row r="564" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F564" s="29"/>
     </row>
-    <row r="565">
+    <row r="565" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F565" s="29"/>
     </row>
-    <row r="566">
+    <row r="566" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F566" s="29"/>
     </row>
-    <row r="567">
+    <row r="567" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F567" s="29"/>
     </row>
-    <row r="568">
+    <row r="568" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F568" s="29"/>
     </row>
-    <row r="569">
+    <row r="569" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F569" s="29"/>
     </row>
-    <row r="570">
+    <row r="570" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F570" s="29"/>
     </row>
-    <row r="571">
+    <row r="571" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F571" s="29"/>
     </row>
-    <row r="572">
+    <row r="572" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F572" s="29"/>
     </row>
-    <row r="573">
+    <row r="573" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F573" s="29"/>
     </row>
-    <row r="574">
+    <row r="574" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F574" s="29"/>
     </row>
-    <row r="575">
+    <row r="575" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F575" s="29"/>
     </row>
-    <row r="576">
+    <row r="576" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F576" s="29"/>
     </row>
-    <row r="577">
+    <row r="577" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F577" s="29"/>
     </row>
-    <row r="578">
+    <row r="578" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F578" s="29"/>
     </row>
-    <row r="579">
+    <row r="579" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F579" s="29"/>
     </row>
-    <row r="580">
+    <row r="580" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F580" s="29"/>
     </row>
-    <row r="581">
+    <row r="581" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F581" s="29"/>
     </row>
-    <row r="582">
+    <row r="582" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F582" s="29"/>
     </row>
-    <row r="583">
+    <row r="583" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F583" s="29"/>
     </row>
-    <row r="584">
+    <row r="584" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F584" s="29"/>
     </row>
-    <row r="585">
+    <row r="585" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F585" s="29"/>
     </row>
-    <row r="586">
+    <row r="586" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F586" s="29"/>
     </row>
-    <row r="587">
+    <row r="587" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F587" s="29"/>
     </row>
-    <row r="588">
+    <row r="588" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F588" s="29"/>
     </row>
-    <row r="589">
+    <row r="589" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F589" s="29"/>
     </row>
-    <row r="590">
+    <row r="590" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F590" s="29"/>
     </row>
-    <row r="591">
+    <row r="591" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F591" s="29"/>
     </row>
-    <row r="592">
+    <row r="592" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F592" s="29"/>
     </row>
-    <row r="593">
+    <row r="593" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F593" s="29"/>
     </row>
-    <row r="594">
+    <row r="594" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F594" s="29"/>
     </row>
-    <row r="595">
+    <row r="595" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F595" s="29"/>
     </row>
-    <row r="596">
+    <row r="596" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F596" s="29"/>
     </row>
-    <row r="597">
+    <row r="597" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F597" s="29"/>
     </row>
-    <row r="598">
+    <row r="598" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F598" s="29"/>
     </row>
-    <row r="599">
+    <row r="599" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F599" s="29"/>
     </row>
-    <row r="600">
+    <row r="600" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F600" s="29"/>
     </row>
-    <row r="601">
+    <row r="601" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F601" s="29"/>
     </row>
-    <row r="602">
+    <row r="602" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F602" s="29"/>
     </row>
-    <row r="603">
+    <row r="603" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F603" s="29"/>
     </row>
-    <row r="604">
+    <row r="604" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F604" s="29"/>
     </row>
-    <row r="605">
+    <row r="605" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F605" s="29"/>
     </row>
-    <row r="606">
+    <row r="606" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F606" s="29"/>
     </row>
-    <row r="607">
+    <row r="607" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F607" s="29"/>
     </row>
-    <row r="608">
+    <row r="608" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F608" s="29"/>
     </row>
-    <row r="609">
+    <row r="609" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F609" s="29"/>
     </row>
-    <row r="610">
+    <row r="610" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F610" s="29"/>
     </row>
-    <row r="611">
+    <row r="611" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F611" s="29"/>
     </row>
-    <row r="612">
+    <row r="612" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F612" s="29"/>
     </row>
-    <row r="613">
+    <row r="613" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F613" s="29"/>
     </row>
-    <row r="614">
+    <row r="614" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F614" s="29"/>
     </row>
-    <row r="615">
+    <row r="615" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F615" s="29"/>
     </row>
-    <row r="616">
+    <row r="616" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F616" s="29"/>
     </row>
-    <row r="617">
+    <row r="617" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F617" s="29"/>
     </row>
-    <row r="618">
+    <row r="618" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F618" s="29"/>
     </row>
-    <row r="619">
+    <row r="619" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F619" s="29"/>
     </row>
-    <row r="620">
+    <row r="620" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F620" s="29"/>
     </row>
-    <row r="621">
+    <row r="621" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F621" s="29"/>
     </row>
-    <row r="622">
+    <row r="622" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F622" s="29"/>
     </row>
-    <row r="623">
+    <row r="623" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F623" s="29"/>
     </row>
-    <row r="624">
+    <row r="624" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F624" s="29"/>
     </row>
-    <row r="625">
+    <row r="625" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F625" s="29"/>
     </row>
-    <row r="626">
+    <row r="626" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F626" s="29"/>
     </row>
-    <row r="627">
+    <row r="627" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F627" s="29"/>
     </row>
-    <row r="628">
+    <row r="628" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F628" s="29"/>
     </row>
-    <row r="629">
+    <row r="629" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F629" s="29"/>
     </row>
-    <row r="630">
+    <row r="630" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F630" s="29"/>
     </row>
-    <row r="631">
+    <row r="631" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F631" s="29"/>
     </row>
-    <row r="632">
+    <row r="632" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F632" s="29"/>
     </row>
-    <row r="633">
+    <row r="633" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F633" s="29"/>
     </row>
-    <row r="634">
+    <row r="634" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F634" s="29"/>
     </row>
-    <row r="635">
+    <row r="635" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F635" s="29"/>
     </row>
-    <row r="636">
+    <row r="636" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F636" s="29"/>
     </row>
-    <row r="637">
+    <row r="637" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F637" s="29"/>
     </row>
-    <row r="638">
+    <row r="638" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F638" s="29"/>
     </row>
-    <row r="639">
+    <row r="639" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F639" s="29"/>
     </row>
-    <row r="640">
+    <row r="640" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F640" s="29"/>
     </row>
-    <row r="641">
+    <row r="641" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F641" s="29"/>
     </row>
-    <row r="642">
+    <row r="642" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F642" s="29"/>
     </row>
-    <row r="643">
+    <row r="643" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F643" s="29"/>
     </row>
-    <row r="644">
+    <row r="644" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F644" s="29"/>
     </row>
-    <row r="645">
+    <row r="645" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F645" s="29"/>
     </row>
-    <row r="646">
+    <row r="646" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F646" s="29"/>
     </row>
-    <row r="647">
+    <row r="647" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F647" s="29"/>
     </row>
-    <row r="648">
+    <row r="648" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F648" s="29"/>
     </row>
-    <row r="649">
+    <row r="649" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F649" s="29"/>
     </row>
-    <row r="650">
+    <row r="650" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F650" s="29"/>
     </row>
-    <row r="651">
+    <row r="651" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F651" s="29"/>
     </row>
-    <row r="652">
+    <row r="652" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F652" s="29"/>
     </row>
-    <row r="653">
+    <row r="653" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F653" s="29"/>
     </row>
-    <row r="654">
+    <row r="654" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F654" s="29"/>
     </row>
-    <row r="655">
+    <row r="655" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F655" s="29"/>
     </row>
-    <row r="656">
+    <row r="656" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F656" s="29"/>
     </row>
-    <row r="657">
+    <row r="657" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F657" s="29"/>
     </row>
-    <row r="658">
+    <row r="658" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F658" s="29"/>
     </row>
-    <row r="659">
+    <row r="659" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F659" s="29"/>
     </row>
-    <row r="660">
+    <row r="660" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F660" s="29"/>
     </row>
-    <row r="661">
+    <row r="661" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F661" s="29"/>
     </row>
-    <row r="662">
+    <row r="662" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F662" s="29"/>
     </row>
-    <row r="663">
+    <row r="663" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F663" s="29"/>
     </row>
-    <row r="664">
+    <row r="664" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F664" s="29"/>
     </row>
-    <row r="665">
+    <row r="665" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F665" s="29"/>
     </row>
-    <row r="666">
+    <row r="666" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F666" s="29"/>
     </row>
-    <row r="667">
+    <row r="667" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F667" s="29"/>
     </row>
-    <row r="668">
+    <row r="668" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F668" s="29"/>
     </row>
-    <row r="669">
+    <row r="669" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F669" s="29"/>
     </row>
-    <row r="670">
+    <row r="670" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F670" s="29"/>
     </row>
-    <row r="671">
+    <row r="671" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F671" s="29"/>
     </row>
-    <row r="672">
+    <row r="672" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F672" s="29"/>
     </row>
-    <row r="673">
+    <row r="673" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F673" s="29"/>
     </row>
-    <row r="674">
+    <row r="674" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F674" s="29"/>
     </row>
-    <row r="675">
+    <row r="675" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F675" s="29"/>
     </row>
-    <row r="676">
+    <row r="676" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F676" s="29"/>
     </row>
-    <row r="677">
+    <row r="677" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F677" s="29"/>
     </row>
-    <row r="678">
+    <row r="678" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F678" s="29"/>
     </row>
-    <row r="679">
+    <row r="679" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F679" s="29"/>
     </row>
-    <row r="680">
+    <row r="680" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F680" s="29"/>
     </row>
-    <row r="681">
+    <row r="681" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F681" s="29"/>
     </row>
-    <row r="682">
+    <row r="682" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F682" s="29"/>
     </row>
-    <row r="683">
+    <row r="683" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F683" s="29"/>
     </row>
-    <row r="684">
+    <row r="684" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F684" s="29"/>
     </row>
-    <row r="685">
+    <row r="685" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F685" s="29"/>
     </row>
-    <row r="686">
+    <row r="686" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F686" s="29"/>
     </row>
-    <row r="687">
+    <row r="687" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F687" s="29"/>
     </row>
-    <row r="688">
+    <row r="688" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F688" s="29"/>
     </row>
-    <row r="689">
+    <row r="689" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F689" s="29"/>
     </row>
-    <row r="690">
+    <row r="690" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F690" s="29"/>
     </row>
-    <row r="691">
+    <row r="691" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F691" s="29"/>
     </row>
-    <row r="692">
+    <row r="692" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F692" s="29"/>
     </row>
-    <row r="693">
+    <row r="693" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F693" s="29"/>
     </row>
-    <row r="694">
+    <row r="694" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F694" s="29"/>
     </row>
-    <row r="695">
+    <row r="695" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F695" s="29"/>
     </row>
-    <row r="696">
+    <row r="696" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F696" s="29"/>
     </row>
-    <row r="697">
+    <row r="697" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F697" s="29"/>
     </row>
-    <row r="698">
+    <row r="698" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F698" s="29"/>
     </row>
-    <row r="699">
+    <row r="699" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F699" s="29"/>
     </row>
-    <row r="700">
+    <row r="700" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F700" s="29"/>
     </row>
-    <row r="701">
+    <row r="701" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F701" s="29"/>
     </row>
-    <row r="702">
+    <row r="702" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F702" s="29"/>
     </row>
-    <row r="703">
+    <row r="703" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F703" s="29"/>
     </row>
-    <row r="704">
+    <row r="704" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F704" s="29"/>
     </row>
-    <row r="705">
+    <row r="705" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F705" s="29"/>
     </row>
-    <row r="706">
+    <row r="706" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F706" s="29"/>
     </row>
-    <row r="707">
+    <row r="707" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F707" s="29"/>
     </row>
-    <row r="708">
+    <row r="708" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F708" s="29"/>
     </row>
-    <row r="709">
+    <row r="709" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F709" s="29"/>
     </row>
-    <row r="710">
+    <row r="710" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F710" s="29"/>
     </row>
-    <row r="711">
+    <row r="711" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F711" s="29"/>
     </row>
-    <row r="712">
+    <row r="712" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F712" s="29"/>
     </row>
-    <row r="713">
+    <row r="713" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F713" s="29"/>
     </row>
-    <row r="714">
+    <row r="714" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F714" s="29"/>
     </row>
-    <row r="715">
+    <row r="715" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F715" s="29"/>
     </row>
-    <row r="716">
+    <row r="716" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F716" s="29"/>
     </row>
-    <row r="717">
+    <row r="717" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F717" s="29"/>
     </row>
-    <row r="718">
+    <row r="718" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F718" s="29"/>
     </row>
-    <row r="719">
+    <row r="719" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F719" s="29"/>
     </row>
-    <row r="720">
+    <row r="720" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F720" s="29"/>
     </row>
-    <row r="721">
+    <row r="721" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F721" s="29"/>
     </row>
-    <row r="722">
+    <row r="722" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F722" s="29"/>
     </row>
-    <row r="723">
+    <row r="723" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F723" s="29"/>
     </row>
-    <row r="724">
+    <row r="724" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F724" s="29"/>
     </row>
-    <row r="725">
+    <row r="725" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F725" s="29"/>
     </row>
-    <row r="726">
+    <row r="726" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F726" s="29"/>
     </row>
-    <row r="727">
+    <row r="727" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F727" s="29"/>
     </row>
-    <row r="728">
+    <row r="728" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F728" s="29"/>
     </row>
-    <row r="729">
+    <row r="729" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F729" s="29"/>
     </row>
-    <row r="730">
+    <row r="730" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F730" s="29"/>
     </row>
-    <row r="731">
+    <row r="731" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F731" s="29"/>
     </row>
-    <row r="732">
+    <row r="732" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F732" s="29"/>
     </row>
-    <row r="733">
+    <row r="733" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F733" s="29"/>
     </row>
-    <row r="734">
+    <row r="734" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F734" s="29"/>
     </row>
-    <row r="735">
+    <row r="735" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F735" s="29"/>
     </row>
-    <row r="736">
+    <row r="736" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F736" s="29"/>
     </row>
-    <row r="737">
+    <row r="737" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F737" s="29"/>
     </row>
-    <row r="738">
+    <row r="738" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F738" s="29"/>
     </row>
-    <row r="739">
+    <row r="739" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F739" s="29"/>
     </row>
-    <row r="740">
+    <row r="740" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F740" s="29"/>
     </row>
-    <row r="741">
+    <row r="741" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F741" s="29"/>
     </row>
-    <row r="742">
+    <row r="742" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F742" s="29"/>
     </row>
-    <row r="743">
+    <row r="743" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F743" s="29"/>
     </row>
-    <row r="744">
+    <row r="744" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F744" s="29"/>
     </row>
-    <row r="745">
+    <row r="745" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F745" s="29"/>
     </row>
-    <row r="746">
+    <row r="746" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F746" s="29"/>
     </row>
-    <row r="747">
+    <row r="747" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F747" s="29"/>
     </row>
-    <row r="748">
+    <row r="748" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F748" s="29"/>
     </row>
-    <row r="749">
+    <row r="749" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F749" s="29"/>
     </row>
-    <row r="750">
+    <row r="750" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F750" s="29"/>
     </row>
-    <row r="751">
+    <row r="751" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F751" s="29"/>
     </row>
-    <row r="752">
+    <row r="752" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F752" s="29"/>
     </row>
-    <row r="753">
+    <row r="753" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F753" s="29"/>
     </row>
-    <row r="754">
+    <row r="754" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F754" s="29"/>
     </row>
-    <row r="755">
+    <row r="755" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F755" s="29"/>
     </row>
-    <row r="756">
+    <row r="756" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F756" s="29"/>
     </row>
-    <row r="757">
+    <row r="757" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F757" s="29"/>
     </row>
-    <row r="758">
+    <row r="758" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F758" s="29"/>
     </row>
-    <row r="759">
+    <row r="759" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F759" s="29"/>
     </row>
-    <row r="760">
+    <row r="760" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F760" s="29"/>
     </row>
-    <row r="761">
+    <row r="761" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F761" s="29"/>
     </row>
-    <row r="762">
+    <row r="762" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F762" s="29"/>
     </row>
-    <row r="763">
+    <row r="763" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F763" s="29"/>
     </row>
-    <row r="764">
+    <row r="764" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F764" s="29"/>
     </row>
-    <row r="765">
+    <row r="765" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F765" s="29"/>
     </row>
-    <row r="766">
+    <row r="766" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F766" s="29"/>
     </row>
-    <row r="767">
+    <row r="767" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F767" s="29"/>
     </row>
-    <row r="768">
+    <row r="768" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F768" s="29"/>
     </row>
-    <row r="769">
+    <row r="769" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F769" s="29"/>
     </row>
-    <row r="770">
+    <row r="770" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F770" s="29"/>
     </row>
-    <row r="771">
+    <row r="771" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F771" s="29"/>
     </row>
-    <row r="772">
+    <row r="772" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F772" s="29"/>
     </row>
-    <row r="773">
+    <row r="773" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F773" s="29"/>
     </row>
-    <row r="774">
+    <row r="774" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F774" s="29"/>
     </row>
-    <row r="775">
+    <row r="775" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F775" s="29"/>
     </row>
-    <row r="776">
+    <row r="776" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F776" s="29"/>
     </row>
-    <row r="777">
+    <row r="777" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F777" s="29"/>
     </row>
-    <row r="778">
+    <row r="778" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F778" s="29"/>
     </row>
-    <row r="779">
+    <row r="779" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F779" s="29"/>
     </row>
-    <row r="780">
+    <row r="780" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F780" s="29"/>
     </row>
-    <row r="781">
+    <row r="781" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F781" s="29"/>
     </row>
-    <row r="782">
+    <row r="782" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F782" s="29"/>
     </row>
-    <row r="783">
+    <row r="783" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F783" s="29"/>
     </row>
-    <row r="784">
+    <row r="784" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F784" s="29"/>
     </row>
-    <row r="785">
+    <row r="785" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F785" s="29"/>
     </row>
-    <row r="786">
+    <row r="786" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F786" s="29"/>
     </row>
-    <row r="787">
+    <row r="787" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F787" s="29"/>
     </row>
-    <row r="788">
+    <row r="788" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F788" s="29"/>
     </row>
-    <row r="789">
+    <row r="789" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F789" s="29"/>
     </row>
-    <row r="790">
+    <row r="790" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F790" s="29"/>
     </row>
-    <row r="791">
+    <row r="791" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F791" s="29"/>
     </row>
-    <row r="792">
+    <row r="792" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F792" s="29"/>
     </row>
-    <row r="793">
+    <row r="793" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F793" s="29"/>
     </row>
-    <row r="794">
+    <row r="794" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F794" s="29"/>
     </row>
-    <row r="795">
+    <row r="795" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F795" s="29"/>
     </row>
-    <row r="796">
+    <row r="796" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F796" s="29"/>
     </row>
-    <row r="797">
+    <row r="797" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F797" s="29"/>
     </row>
-    <row r="798">
+    <row r="798" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F798" s="29"/>
     </row>
-    <row r="799">
+    <row r="799" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F799" s="29"/>
     </row>
-    <row r="800">
+    <row r="800" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F800" s="29"/>
     </row>
-    <row r="801">
+    <row r="801" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F801" s="29"/>
     </row>
-    <row r="802">
+    <row r="802" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F802" s="29"/>
     </row>
-    <row r="803">
+    <row r="803" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F803" s="29"/>
     </row>
-    <row r="804">
+    <row r="804" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F804" s="29"/>
     </row>
-    <row r="805">
+    <row r="805" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F805" s="29"/>
     </row>
-    <row r="806">
+    <row r="806" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F806" s="29"/>
     </row>
-    <row r="807">
+    <row r="807" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F807" s="29"/>
     </row>
-    <row r="808">
+    <row r="808" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F808" s="29"/>
     </row>
-    <row r="809">
+    <row r="809" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F809" s="29"/>
     </row>
-    <row r="810">
+    <row r="810" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F810" s="29"/>
     </row>
-    <row r="811">
+    <row r="811" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F811" s="29"/>
     </row>
-    <row r="812">
+    <row r="812" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F812" s="29"/>
     </row>
-    <row r="813">
+    <row r="813" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F813" s="29"/>
     </row>
-    <row r="814">
+    <row r="814" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F814" s="29"/>
     </row>
-    <row r="815">
+    <row r="815" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F815" s="29"/>
     </row>
-    <row r="816">
+    <row r="816" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F816" s="29"/>
     </row>
-    <row r="817">
+    <row r="817" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F817" s="29"/>
     </row>
-    <row r="818">
+    <row r="818" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F818" s="29"/>
     </row>
-    <row r="819">
+    <row r="819" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F819" s="29"/>
     </row>
-    <row r="820">
+    <row r="820" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F820" s="29"/>
     </row>
-    <row r="821">
+    <row r="821" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F821" s="29"/>
     </row>
-    <row r="822">
+    <row r="822" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F822" s="29"/>
     </row>
-    <row r="823">
+    <row r="823" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F823" s="29"/>
     </row>
-    <row r="824">
+    <row r="824" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F824" s="29"/>
     </row>
-    <row r="825">
+    <row r="825" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F825" s="29"/>
     </row>
-    <row r="826">
+    <row r="826" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F826" s="29"/>
     </row>
-    <row r="827">
+    <row r="827" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F827" s="29"/>
     </row>
-    <row r="828">
+    <row r="828" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F828" s="29"/>
     </row>
-    <row r="829">
+    <row r="829" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F829" s="29"/>
     </row>
-    <row r="830">
+    <row r="830" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F830" s="29"/>
     </row>
-    <row r="831">
+    <row r="831" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F831" s="29"/>
     </row>
-    <row r="832">
+    <row r="832" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F832" s="29"/>
     </row>
-    <row r="833">
+    <row r="833" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F833" s="29"/>
     </row>
-    <row r="834">
+    <row r="834" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F834" s="29"/>
     </row>
-    <row r="835">
+    <row r="835" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F835" s="29"/>
     </row>
-    <row r="836">
+    <row r="836" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F836" s="29"/>
     </row>
-    <row r="837">
+    <row r="837" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F837" s="29"/>
     </row>
-    <row r="838">
+    <row r="838" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F838" s="29"/>
     </row>
-    <row r="839">
+    <row r="839" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F839" s="29"/>
     </row>
-    <row r="840">
+    <row r="840" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F840" s="29"/>
     </row>
-    <row r="841">
+    <row r="841" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F841" s="29"/>
     </row>
-    <row r="842">
+    <row r="842" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F842" s="29"/>
     </row>
-    <row r="843">
+    <row r="843" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F843" s="29"/>
     </row>
-    <row r="844">
+    <row r="844" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F844" s="29"/>
     </row>
-    <row r="845">
+    <row r="845" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F845" s="29"/>
     </row>
-    <row r="846">
+    <row r="846" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F846" s="29"/>
     </row>
-    <row r="847">
+    <row r="847" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F847" s="29"/>
     </row>
-    <row r="848">
+    <row r="848" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F848" s="29"/>
     </row>
-    <row r="849">
+    <row r="849" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F849" s="29"/>
     </row>
-    <row r="850">
+    <row r="850" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F850" s="29"/>
     </row>
-    <row r="851">
+    <row r="851" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F851" s="29"/>
     </row>
-    <row r="852">
+    <row r="852" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F852" s="29"/>
     </row>
-    <row r="853">
+    <row r="853" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F853" s="29"/>
     </row>
-    <row r="854">
+    <row r="854" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F854" s="29"/>
     </row>
-    <row r="855">
+    <row r="855" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F855" s="29"/>
     </row>
-    <row r="856">
+    <row r="856" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F856" s="29"/>
     </row>
-    <row r="857">
+    <row r="857" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F857" s="29"/>
     </row>
-    <row r="858">
+    <row r="858" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F858" s="29"/>
     </row>
-    <row r="859">
+    <row r="859" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F859" s="29"/>
     </row>
-    <row r="860">
+    <row r="860" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F860" s="29"/>
     </row>
-    <row r="861">
+    <row r="861" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F861" s="29"/>
     </row>
-    <row r="862">
+    <row r="862" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F862" s="29"/>
     </row>
-    <row r="863">
+    <row r="863" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F863" s="29"/>
     </row>
-    <row r="864">
+    <row r="864" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F864" s="29"/>
     </row>
-    <row r="865">
+    <row r="865" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F865" s="29"/>
     </row>
-    <row r="866">
+    <row r="866" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F866" s="29"/>
     </row>
-    <row r="867">
+    <row r="867" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F867" s="29"/>
     </row>
-    <row r="868">
+    <row r="868" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F868" s="29"/>
     </row>
-    <row r="869">
+    <row r="869" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F869" s="29"/>
     </row>
-    <row r="870">
+    <row r="870" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F870" s="29"/>
     </row>
-    <row r="871">
+    <row r="871" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F871" s="29"/>
     </row>
-    <row r="872">
+    <row r="872" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F872" s="29"/>
     </row>
-    <row r="873">
+    <row r="873" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F873" s="29"/>
     </row>
-    <row r="874">
+    <row r="874" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F874" s="29"/>
     </row>
-    <row r="875">
+    <row r="875" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F875" s="29"/>
     </row>
-    <row r="876">
+    <row r="876" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F876" s="29"/>
     </row>
-    <row r="877">
+    <row r="877" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F877" s="29"/>
     </row>
-    <row r="878">
+    <row r="878" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F878" s="29"/>
     </row>
-    <row r="879">
+    <row r="879" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F879" s="29"/>
     </row>
-    <row r="880">
+    <row r="880" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F880" s="29"/>
     </row>
-    <row r="881">
+    <row r="881" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F881" s="29"/>
     </row>
-    <row r="882">
+    <row r="882" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F882" s="29"/>
     </row>
-    <row r="883">
+    <row r="883" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F883" s="29"/>
     </row>
-    <row r="884">
+    <row r="884" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F884" s="29"/>
     </row>
-    <row r="885">
+    <row r="885" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F885" s="29"/>
     </row>
-    <row r="886">
+    <row r="886" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F886" s="29"/>
     </row>
-    <row r="887">
+    <row r="887" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F887" s="29"/>
     </row>
-    <row r="888">
+    <row r="888" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F888" s="29"/>
     </row>
-    <row r="889">
+    <row r="889" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F889" s="29"/>
     </row>
-    <row r="890">
+    <row r="890" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F890" s="29"/>
     </row>
-    <row r="891">
+    <row r="891" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F891" s="29"/>
     </row>
-    <row r="892">
+    <row r="892" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F892" s="29"/>
     </row>
-    <row r="893">
+    <row r="893" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F893" s="29"/>
     </row>
-    <row r="894">
+    <row r="894" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F894" s="29"/>
     </row>
-    <row r="895">
+    <row r="895" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F895" s="29"/>
     </row>
-    <row r="896">
+    <row r="896" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F896" s="29"/>
     </row>
-    <row r="897">
+    <row r="897" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F897" s="29"/>
     </row>
-    <row r="898">
+    <row r="898" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F898" s="29"/>
     </row>
-    <row r="899">
+    <row r="899" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F899" s="29"/>
     </row>
-    <row r="900">
+    <row r="900" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F900" s="29"/>
     </row>
-    <row r="901">
+    <row r="901" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F901" s="29"/>
     </row>
-    <row r="902">
+    <row r="902" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F902" s="29"/>
     </row>
-    <row r="903">
+    <row r="903" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F903" s="29"/>
     </row>
-    <row r="904">
+    <row r="904" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F904" s="29"/>
     </row>
-    <row r="905">
+    <row r="905" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F905" s="29"/>
     </row>
-    <row r="906">
+    <row r="906" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F906" s="29"/>
     </row>
-    <row r="907">
+    <row r="907" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F907" s="29"/>
     </row>
-    <row r="908">
+    <row r="908" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F908" s="29"/>
     </row>
-    <row r="909">
+    <row r="909" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F909" s="29"/>
     </row>
-    <row r="910">
+    <row r="910" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F910" s="29"/>
     </row>
-    <row r="911">
+    <row r="911" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F911" s="29"/>
     </row>
-    <row r="912">
+    <row r="912" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F912" s="29"/>
     </row>
-    <row r="913">
+    <row r="913" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F913" s="29"/>
     </row>
-    <row r="914">
+    <row r="914" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F914" s="29"/>
     </row>
-    <row r="915">
+    <row r="915" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F915" s="29"/>
     </row>
-    <row r="916">
+    <row r="916" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F916" s="29"/>
     </row>
-    <row r="917">
+    <row r="917" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F917" s="29"/>
     </row>
-    <row r="918">
+    <row r="918" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F918" s="29"/>
     </row>
-    <row r="919">
+    <row r="919" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F919" s="29"/>
     </row>
-    <row r="920">
+    <row r="920" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F920" s="29"/>
     </row>
-    <row r="921">
+    <row r="921" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F921" s="29"/>
     </row>
-    <row r="922">
+    <row r="922" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F922" s="29"/>
     </row>
-    <row r="923">
+    <row r="923" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F923" s="29"/>
     </row>
-    <row r="924">
+    <row r="924" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F924" s="29"/>
     </row>
-    <row r="925">
+    <row r="925" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F925" s="29"/>
     </row>
-    <row r="926">
+    <row r="926" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F926" s="29"/>
     </row>
-    <row r="927">
+    <row r="927" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F927" s="29"/>
     </row>
-    <row r="928">
+    <row r="928" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F928" s="29"/>
     </row>
-    <row r="929">
+    <row r="929" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F929" s="29"/>
     </row>
-    <row r="930">
+    <row r="930" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F930" s="29"/>
     </row>
-    <row r="931">
+    <row r="931" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F931" s="29"/>
     </row>
-    <row r="932">
+    <row r="932" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F932" s="29"/>
     </row>
-    <row r="933">
+    <row r="933" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F933" s="29"/>
     </row>
-    <row r="934">
+    <row r="934" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F934" s="29"/>
     </row>
-    <row r="935">
+    <row r="935" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F935" s="29"/>
     </row>
-    <row r="936">
+    <row r="936" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F936" s="29"/>
     </row>
-    <row r="937">
+    <row r="937" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F937" s="29"/>
     </row>
-    <row r="938">
+    <row r="938" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F938" s="29"/>
     </row>
-    <row r="939">
+    <row r="939" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F939" s="29"/>
     </row>
-    <row r="940">
+    <row r="940" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F940" s="29"/>
     </row>
-    <row r="941">
+    <row r="941" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F941" s="29"/>
     </row>
-    <row r="942">
+    <row r="942" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F942" s="29"/>
     </row>
-    <row r="943">
+    <row r="943" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F943" s="29"/>
     </row>
-    <row r="944">
+    <row r="944" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F944" s="29"/>
     </row>
-    <row r="945">
+    <row r="945" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F945" s="29"/>
     </row>
-    <row r="946">
+    <row r="946" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F946" s="29"/>
     </row>
-    <row r="947">
+    <row r="947" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F947" s="29"/>
     </row>
-    <row r="948">
+    <row r="948" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F948" s="29"/>
     </row>
-    <row r="949">
+    <row r="949" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F949" s="29"/>
     </row>
-    <row r="950">
+    <row r="950" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F950" s="29"/>
     </row>
-    <row r="951">
+    <row r="951" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F951" s="29"/>
     </row>
-    <row r="952">
+    <row r="952" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F952" s="29"/>
     </row>
-    <row r="953">
+    <row r="953" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F953" s="29"/>
     </row>
-    <row r="954">
+    <row r="954" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F954" s="29"/>
     </row>
-    <row r="955">
+    <row r="955" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F955" s="29"/>
     </row>
-    <row r="956">
+    <row r="956" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F956" s="29"/>
     </row>
-    <row r="957">
+    <row r="957" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F957" s="29"/>
     </row>
-    <row r="958">
+    <row r="958" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F958" s="29"/>
     </row>
-    <row r="959">
+    <row r="959" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F959" s="29"/>
     </row>
-    <row r="960">
+    <row r="960" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F960" s="29"/>
     </row>
-    <row r="961">
+    <row r="961" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F961" s="29"/>
     </row>
-    <row r="962">
+    <row r="962" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F962" s="29"/>
     </row>
-    <row r="963">
+    <row r="963" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F963" s="29"/>
     </row>
-    <row r="964">
+    <row r="964" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F964" s="29"/>
     </row>
-    <row r="965">
+    <row r="965" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F965" s="29"/>
     </row>
-    <row r="966">
+    <row r="966" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F966" s="29"/>
     </row>
-    <row r="967">
+    <row r="967" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F967" s="29"/>
     </row>
-    <row r="968">
+    <row r="968" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F968" s="29"/>
     </row>
-    <row r="969">
+    <row r="969" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F969" s="29"/>
     </row>
-    <row r="970">
+    <row r="970" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F970" s="29"/>
     </row>
-    <row r="971">
+    <row r="971" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F971" s="29"/>
     </row>
-    <row r="972">
+    <row r="972" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F972" s="29"/>
     </row>
-    <row r="973">
+    <row r="973" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F973" s="29"/>
     </row>
-    <row r="974">
+    <row r="974" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F974" s="29"/>
     </row>
-    <row r="975">
+    <row r="975" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F975" s="29"/>
     </row>
-    <row r="976">
+    <row r="976" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F976" s="29"/>
     </row>
-    <row r="977">
+    <row r="977" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F977" s="29"/>
     </row>
-    <row r="978">
+    <row r="978" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F978" s="29"/>
     </row>
-    <row r="979">
+    <row r="979" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F979" s="29"/>
     </row>
-    <row r="980">
+    <row r="980" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F980" s="29"/>
     </row>
-    <row r="981">
+    <row r="981" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F981" s="29"/>
     </row>
-    <row r="982">
+    <row r="982" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F982" s="29"/>
     </row>
-    <row r="983">
+    <row r="983" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F983" s="29"/>
     </row>
-    <row r="984">
+    <row r="984" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F984" s="29"/>
     </row>
-    <row r="985">
+    <row r="985" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F985" s="29"/>
     </row>
-    <row r="986">
+    <row r="986" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F986" s="29"/>
     </row>
-    <row r="987">
+    <row r="987" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F987" s="29"/>
     </row>
-    <row r="988">
+    <row r="988" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F988" s="29"/>
     </row>
-    <row r="989">
+    <row r="989" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F989" s="29"/>
     </row>
-    <row r="990">
+    <row r="990" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F990" s="29"/>
     </row>
-    <row r="991">
+    <row r="991" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F991" s="29"/>
     </row>
-    <row r="992">
+    <row r="992" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F992" s="29"/>
     </row>
-    <row r="993">
+    <row r="993" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F993" s="29"/>
     </row>
-    <row r="994">
+    <row r="994" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F994" s="29"/>
     </row>
-    <row r="995">
+    <row r="995" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F995" s="29"/>
     </row>
   </sheetData>
@@ -3668,11 +3943,11 @@
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A26:F26"/>
   </mergeCells>
-  <dataValidations>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="E8">
       <formula1>"150000,200000"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>